<commit_message>
updated harmonic similarity link files
</commit_message>
<xml_diff>
--- a/hsim-experiment/harmonic_similarity_split_link/harmonic_similarity_matches_1.xlsx
+++ b/hsim-experiment/harmonic_similarity_split_link/harmonic_similarity_matches_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,45 +436,50 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>similarity_range</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>track_1</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>track_2</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>sim_val</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>pattern_track_1</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>pattern_track_2</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>time_pattern_track_1</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>time_pattern_track_2</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>link_track_1</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>link_track_2</t>
         </is>
@@ -483,722 +488,676 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>schubert-winterreise_28</t>
+          <t>mid</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>schubert-winterreise_203</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0.2657342657342657</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>[['A:maj/E', 'E:7', 'A:maj', 'E:7', 'A:maj']]</t>
-        </is>
+          <t>isophonics_265</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>isophonics_298</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.4903846153846154</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[['G:maj', 'D:7/C', 'G:maj/B', 'D:7/C', 'G:maj/B']]</t>
+          <t>[['A', 'D', 'A']]</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[(15.3, 19.72)]</t>
+          <t>[['G', 'C', 'G']]</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[(68.82, 84.54)]</t>
+          <t>[('0:01:45.425056', '0:01:55.003287')]</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>spotify:track:0XfunCHFEeQnzm4NaY8rJr</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>spotify:track:68YORkKP9uvlOQFMZZZwH5</t>
-        </is>
-      </c>
+          <t>[('0:00:00.344657', '0:00:11.337709')]</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>schubert-winterreise_157</t>
+          <t>hi</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>isophonics_3</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>0.1187888198757764</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>[['F:maj', 'C:maj', 'F:maj']]</t>
-        </is>
+          <t>schubert-winterreise_125</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_76</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[['G', 'D', 'G']]</t>
+          <t>[['E:(3,b5,b7)/G#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#']]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[(40.96, 43.3)]</t>
+          <t>[['D#:(3,b5,b7)/G', 'G#:maj', 'D#:(3,b5,b7)/A', 'G#:maj', 'D#:(3,b5,b7)/A', 'G#:maj', 'D#:(3,b5,b7)/A', 'G#:maj', 'D#:(3,b5,b7)/A', 'G#:maj', 'D#:(3,b5,b7)/A']]</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>[(1.014823, 6.126439)]</t>
+          <t>[('0:00:48.440000', '0:00:53.480000')]</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>spotify:track:4lrfYSnZmpXdCWuWqVo8L0</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>spotify:track:68BTFws92cRztMS1oQ7Ewj</t>
-        </is>
-      </c>
+          <t>[('0:00:55.560000', '0:01:00.520000')]</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>schubert-winterreise_149</t>
+          <t>mid</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>schubert-winterreise_184</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>[['A:min', 'B:hdim7/D', 'E:7', 'A:min', 'A:min', 'B:hdim7/D', 'E:7', 'A:min', 'G#:dim7', 'A:min', 'G#:dim7', 'E:maj/B', 'A:min/C', 'G:maj/B', 'F:maj/A', 'C:maj/G', 'F:maj', 'C:maj/G', 'G:7', 'C:maj', 'F:maj/A', 'E:min/B', 'B:7', 'E:min', 'D#:dim7/F#', 'E:min/G', 'E:(3,5,b7,b9)/G#', 'A:min', 'A:(3,5,b7,b9)', 'D:min', 'A:min/E', 'E:(3,5,b7,b9)', 'G#:dim7', 'B:hdim7/D', 'G#:dim7', 'B:hdim7/D', 'E:(3,5,b7,b9)', 'A:min', 'A:(3,5,b7,b9)/C#', 'D:min', 'A:min/E', 'E:(3,5,b7,b9)', 'A:min']]</t>
-        </is>
+          <t>schubert-winterreise_21</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_124</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.3736263736263736</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[['G:min', 'A:hdim7/C', 'D:7', 'G:min', 'G:min', 'A:hdim7/C', 'D:7', 'G:min', 'F#:dim7', 'G:min', 'F#:dim7', 'D:maj/A', 'G:min/A#', 'F:maj/A', 'D#:maj/G', 'A#:maj/F', 'D#:maj', 'A#:maj/F', 'F:7', 'A#:maj', 'D#:maj/G', 'D:min/A', 'A:7', 'D:min', 'C#:dim7/E', 'D:min/F', 'D:(3,5,b7,b9)/F#', 'G:min', 'G:(3,5,b7,b9)', 'C:min', 'G:min/D', 'D:(3,5,b7,b9)', 'F#:dim7', 'A:hdim7/C', 'F#:dim7', 'A:hdim7/C', 'D:(3,5,b7,b9)', 'G:min', 'G:(3,5,b7,b9)/B', 'C:min', 'G:min/D', 'D:(3,5,b7,b9)', 'G:min']]</t>
+          <t>[['A#:maj', 'D#:min', 'A#:maj', 'D#:min', 'A#:maj', 'D#:min']]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[(10.56, 69.42)]</t>
+          <t>[['C', 'F:min/C', 'C', 'F:min', 'C', 'F:min']]</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>[(9.18, 61.0)]</t>
+          <t>[('0:00:02.020000', '0:00:10.620000')]</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>spotify:track:2qCvEz2hEb92VFATqVvrht</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>spotify:track:2qCvEz2hEb92VFATqVvrht</t>
-        </is>
-      </c>
+          <t>[('0:00:49.480000', '0:01:02.360000')]</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>schubert-winterreise_177</t>
+          <t>low</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>schubert-winterreise_65</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>0.1384615384615385</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>[['A:min/E', 'E:7', 'A:min'], ['A:min', 'E:maj', 'A:min']]</t>
-        </is>
+          <t>schubert-winterreise_15</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_62</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.2666666666666667</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[['D#:min', 'A#:7', 'D#:min'], ['D#:min', 'A#:maj', 'D#:min']]</t>
+          <t>[['F:7', 'A#:maj/F', 'F:7', 'A#:maj']]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[(83.1, 90.02), (13.5, 21.9)]</t>
+          <t>[['F:7', 'A#:maj/F', 'F:7', 'A#:maj/F']]</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>[(9.1, 13.86), (0.78, 5.98)]</t>
+          <t>[('0:01:34.060000', '0:01:45.580000')]</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>spotify:track:2g41AZ58LFdQLxmWx82ujI</t>
+          <t>[('0:01:30.140000', '0:01:38.780000')]</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>spotify:track:1nvxQGWCnikMK7a4HYQvSx</t>
+          <t>spotify:track:3OD2uwEUQKg0WyW9Lewata</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>spotify:track:1yerCi2iQCVkdHG6rdRn7R</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>schubert-winterreise_137</t>
+          <t>mid</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>schubert-winterreise_0</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0.1846153846153846</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>[['E:7', 'A:min', 'D:min', 'A:min']]</t>
-        </is>
+          <t>schubert-winterreise_59</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_203</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.4211538461538462</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>[['F#:7/B', 'B:min', 'E:min/B', 'B:min']]</t>
+          <t>[['B:7', 'E:maj', 'B:7', 'E:maj', 'B:7', 'E:maj']]</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>[(49.06, 59.7)]</t>
+          <t>[['D:7', 'G:maj', 'D:7/C', 'G:maj/B', 'D:7/C', 'G:maj/B']]</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>[(23.02, 32.58)]</t>
+          <t>[('0:00:17.180000', '0:00:48.160000')]</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>spotify:track:3OD2uwEUQKg0WyW9Lewata</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>spotify:track:2g41AZ58LFdQLxmWx82ujI</t>
+          <t>[('0:01:06.920000', '0:01:24.540000')]</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>spotify:track:68YORkKP9uvlOQFMZZZwH5</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>isophonics_14</t>
+          <t>low</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>schubert-winterreise_128</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>0.06995192307692308</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>[['C:7', 'F', 'C/3']]</t>
-        </is>
+          <t>schubert-winterreise_20</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_26</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.2</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[['G:7/F', 'C:maj/E', 'G:maj/D']]</t>
+          <t>[['B:min', 'F#:7/A#', 'B:min']]</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[(12.503707, 19.759943)]</t>
+          <t>[['F:min', 'C:7', 'F:min']]</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>[(65.64, 70.54)]</t>
+          <t>[('0:00:39.040000', '0:00:46.100000')]</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>spotify:track:0pNeVovbiZHkulpGeOx1Gj</t>
+          <t>[('0:00:09.620000', '0:00:14.180000')]</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>spotify:track:68YORkKP9uvlOQFMZZZwH5</t>
+          <t>spotify:track:1yerCi2iQCVkdHG6rdRn7R</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>spotify:track:1nvxQGWCnikMK7a4HYQvSx</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>schubert-winterreise_169</t>
+          <t>hi</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>schubert-winterreise_110</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>0.2666666666666667</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>[['D#:7', 'G#:maj/D#', 'D#:7', 'G#:maj']]</t>
-        </is>
+          <t>schubert-winterreise_53</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_148</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.7083333333333333</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>[['G:7', 'C:maj/G', 'G:7', 'C:maj/G']]</t>
+          <t>[['B:7', 'E:maj', 'B:7', 'E:maj', 'B:7', 'E:maj']]</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>[(108.54, 120.72)]</t>
+          <t>[['D:7', 'G:maj', 'D:7', 'G:maj', 'D:7', 'G:maj']]</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>[(88.86, 97.74)]</t>
+          <t>[('0:00:15.260000', '0:00:45.460000')]</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>spotify:track:3OD2uwEUQKg0WyW9Lewata</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>spotify:track:1yerCi2iQCVkdHG6rdRn7R</t>
-        </is>
-      </c>
+          <t>[('0:00:36.320000', '0:00:51.920000')]</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>schubert-winterreise_188</t>
+          <t>mid</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>schubert-winterreise_171</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>0.2202898550724638</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>[['A#:min', 'F:min', 'C:7', 'F:min']]</t>
-        </is>
+          <t>schubert-winterreise_40</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_33</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.4017857142857143</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>[['B:min/F#', 'F#:min', 'C#:7', 'F#:min']]</t>
+          <t>[['D:maj', 'A:7', 'D:maj'], ['D:maj/F#', 'G:maj', 'D:maj']]</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>[(7.8, 13.9)]</t>
+          <t>[['G:maj/D', 'D:7', 'G:maj'], ['G:maj/B', 'C:maj', 'G:maj/D']]</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>[(2.68, 6.46)]</t>
+          <t>[('0:00:02.360000', '0:00:11.660000'), ('0:01:00.040000', '0:01:07.080000')]</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>spotify:track:1nvxQGWCnikMK7a4HYQvSx</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>spotify:track:4lrfYSnZmpXdCWuWqVo8L0</t>
-        </is>
-      </c>
+          <t>[('0:01:05.440000', '0:01:06.820000'), ('0:01:03.600000', '0:01:06.040000')]</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>schubert-winterreise_15</t>
+          <t>mid</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>schubert-winterreise_7</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>0.1348837209302326</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>[['E:7', 'A:min', 'A:min']]</t>
-        </is>
+          <t>schubert-winterreise_151</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>isophonics_151</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.4</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>[['E:7', 'A:min', 'A:min']]</t>
+          <t>[['F:maj', 'C:maj/G', 'F:maj/A'], ['C:maj/G', 'F:maj', 'C:maj/G']]</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>[(7.36, 16.52)]</t>
+          <t>[['Bb', 'F', 'Bb'], ['F', 'Bb', 'F']]</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>[(14.78, 19.02)]</t>
+          <t>[('0:02:00', '0:02:02.700000'), ('0:01:57.540000', '0:02:01.800000')]</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>spotify:track:3OD2uwEUQKg0WyW9Lewata</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>spotify:track:2qCvEz2hEb92VFATqVvrht</t>
-        </is>
-      </c>
+          <t>[('0:00:22.564557', '0:00:26.651269'), ('0:00:23.586235', '0:00:28.578526')]</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>schubert-winterreise_109</t>
+          <t>low</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>schubert-winterreise_43</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
+          <t>schubert-winterreise_152</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_113</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
         <v>0.1348837209302326</v>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>[['D:min', 'A:7/E', 'D:min']]</t>
-        </is>
-      </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>[['B:min', 'F#:7/A#', 'B:min']]</t>
+          <t>[['E:7', 'A:min', 'A:min']]</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>[(1.54, 6.88)]</t>
+          <t>[['C:7', 'F:min/C', 'F:min']]</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>[(41.32, 48.94)]</t>
+          <t>[('0:00:13.660000', '0:00:17.900000')]</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>spotify:track:5UYEp9kllA47IhttiiMuJ0</t>
+          <t>[('0:00:34.560000', '0:00:36.420000')]</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>spotify:track:1yerCi2iQCVkdHG6rdRn7R</t>
+          <t>spotify:track:2qCvEz2hEb92VFATqVvrht</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>spotify:track:1nvxQGWCnikMK7a4HYQvSx</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>schubert-winterreise_156</t>
+          <t>low</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>schubert-winterreise_106</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>0.1652173913043478</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>[['F#:min', 'C#:7', 'F#:min']]</t>
-        </is>
+          <t>schubert-winterreise_5</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_163</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.1348837209302326</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>[['B:min', 'F#:7/A#', 'B:min']]</t>
+          <t>[['E:7', 'A:min', 'A:min']]</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>[(3.32, 6.3)]</t>
+          <t>[['C:7', 'F:min/C', 'F:min']]</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>[(39.84, 47.28)]</t>
+          <t>[('0:00:13.600000', '0:00:17.780000')]</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>spotify:track:4lrfYSnZmpXdCWuWqVo8L0</t>
+          <t>[('0:00:32.320000', '0:00:33.880000')]</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>spotify:track:1yerCi2iQCVkdHG6rdRn7R</t>
+          <t>spotify:track:2qCvEz2hEb92VFATqVvrht</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>spotify:track:1nvxQGWCnikMK7a4HYQvSx</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>schubert-winterreise_173</t>
+          <t>hi</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>schubert-winterreise_2</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>0.2687747035573123</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>[['D:7', 'G:maj', 'G:maj/B', 'D:7']]</t>
-        </is>
+          <t>schubert-winterreise_131</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_42</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.7142857142857143</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>[['E:7', 'A:maj', 'A:maj', 'E:7/G#']]</t>
+          <t>[['D#:maj/A#', 'A#:(3,5,b7,b9)', 'D#:maj']]</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>[(18.3, 21.32)]</t>
+          <t>[['G#:maj', 'D#:(3,5,b7,b9)', 'G#:maj']]</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>[(8.34, 16.5)]</t>
+          <t>[('0:00:57.420000', '0:01:00.320000')]</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>spotify:track:4lrfYSnZmpXdCWuWqVo8L0</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>spotify:track:0XfunCHFEeQnzm4NaY8rJr</t>
-        </is>
-      </c>
+          <t>[('0:00:20.540000', '0:00:23.160000')]</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>schubert-winterreise_61</t>
+          <t>low</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>schubert-winterreise_65</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>0.2461538461538462</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>[['D:7', 'G:maj', 'D:7/C', 'G:maj/B', 'D:7/C', 'G:maj/B']]</t>
-        </is>
+          <t>schubert-winterreise_157</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_45</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.1652173913043478</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>[['A#:7', 'D#:maj', 'A#:7', 'D#:maj', 'A#:7', 'D#:maj']]</t>
+          <t>[['F:min', 'C:7', 'F:min']]</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>[(68.98, 87.2)]</t>
+          <t>[['B:min', 'F#:7/A#', 'B:min']]</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>[(120.66, 122.74)]</t>
+          <t>[('0:00:02.560000', '0:00:04.800000')]</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>spotify:track:68YORkKP9uvlOQFMZZZwH5</t>
+          <t>[('0:00:36.660000', '0:00:43.940000')]</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>spotify:track:1nvxQGWCnikMK7a4HYQvSx</t>
+          <t>spotify:track:4lrfYSnZmpXdCWuWqVo8L0</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>spotify:track:1yerCi2iQCVkdHG6rdRn7R</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>schubert-winterreise_89</t>
+          <t>hi</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>schubert-winterreise_205</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>0.1177257525083612</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>[['C:min/G', 'G:min', 'D:7', 'G:min']]</t>
-        </is>
+          <t>schubert-winterreise_201</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_204</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>[['C:min/D#', 'G:min/D', 'D:7', 'G:min']]</t>
+          <t>[['D:(3,b5,b7)/F#', 'G:maj', 'D:(3,b5,b7)/G#', 'G:maj', 'D:(3,b5,b7)/G#', 'G:maj', 'D:(3,b5,b7)/G#', 'G:maj', 'D:(3,b5,b7)/G#', 'G:maj', 'D:(3,b5,b7)/G#']]</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>[(2.98, 6.7)]</t>
+          <t>[['E:(3,b5,b7)/G#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#', 'A:maj', 'E:(3,b5,b7)/A#']]</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>[(41.3, 43.48)]</t>
+          <t>[('0:00:37.820000', '0:00:42.820000')]</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>spotify:track:4lrfYSnZmpXdCWuWqVo8L0</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>spotify:track:68YORkKP9uvlOQFMZZZwH5</t>
-        </is>
-      </c>
+          <t>[('0:00:43.100000', '0:00:47.740000')]</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>isophonics_82</t>
+          <t>hi</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>schubert-winterreise_205</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>0.05499181669394435</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>[['A', 'D', 'A']]</t>
-        </is>
+          <t>schubert-winterreise_81</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>schubert-winterreise_133</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.7142857142857143</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[['G:maj', 'C:maj/G', 'G:maj']]</t>
+          <t>[['A#:maj', 'F:(3,5,b7,b9)', 'A#:maj']]</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>[(3.988594, 7.754783)]</t>
+          <t>[['D#:maj/A#', 'A#:(3,5,b7,b9)', 'D#:maj']]</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>[(16.92, 23.9)]</t>
+          <t>[('0:00:19.260000', '0:00:22.260000')]</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>spotify:track:5EzvwjFwdP5Kfl5AZAemzu</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>spotify:track:68YORkKP9uvlOQFMZZZwH5</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>schubert-winterreise_19</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>schubert-winterreise_184</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>0.06976744186046512</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>[['A:7', 'D:min', 'D:min'], ['F:maj/C', 'C:7', 'F:maj']]</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>[['D:7', 'G:min', 'G:min'], ['A#:maj/F', 'F:7', 'A#:maj']]</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>[(9.64, 22.68), (66.22, 72.3)]</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>[(11.62, 15.6), (28.02, 30.1)]</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>spotify:track:5UYEp9kllA47IhttiiMuJ0</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>spotify:track:2qCvEz2hEb92VFATqVvrht</t>
-        </is>
-      </c>
+          <t>[('0:00:57.920000', '0:01:00.680000')]</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>